<commit_message>
B21_Cucumber and JUnit Files
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekchicago-1/Desktop/cybertek21-cucumber-junit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asiabizub/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D33B20-A88F-8945-AA53-A3B7997FC859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F3CB33-7965-7A41-B7BE-3FD9BF15823F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{973C79E2-212B-7C44-A95E-272F10C99F5C}"/>
+    <workbookView xWindow="-33500" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{B9D594BA-CA76-3044-BED9-4E37CA6C98DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FirstName</t>
   </si>
@@ -39,10 +42,19 @@
     <t>LastName</t>
   </si>
   <si>
+    <t xml:space="preserve">Asia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bizub </t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
     <t>JOB_ID</t>
   </si>
   <si>
-    <t>Steven</t>
+    <t xml:space="preserve">Steven </t>
   </si>
   <si>
     <t>King</t>
@@ -51,44 +63,28 @@
     <t>President</t>
   </si>
   <si>
+    <t xml:space="preserve">Adam </t>
+  </si>
+  <si>
     <t>Sandler</t>
   </si>
   <si>
-    <t>Adam</t>
-  </si>
-  <si>
     <t>Actor</t>
   </si>
   <si>
-    <t>Ricky</t>
+    <t xml:space="preserve">Ricky </t>
   </si>
   <si>
     <t>Martin</t>
   </si>
   <si>
     <t>Singer</t>
-  </si>
-  <si>
-    <t>Neena</t>
-  </si>
-  <si>
-    <t>Kochar</t>
-  </si>
-  <si>
-    <t>SDET</t>
-  </si>
-  <si>
-    <t>Madam</t>
-  </si>
-  <si>
-    <t>Tom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -433,11 +429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703330C3-72DB-6E40-99AA-6839C2873A25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F167B283-C841-9A4A-9446-148FD39F8BB4}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,26 +446,26 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>

</xml_diff>